<commit_message>
resultados preliminares golden rule
</commit_message>
<xml_diff>
--- a/GDP/simple_golden_rule_pan.xlsx
+++ b/GDP/simple_golden_rule_pan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana-my.sharepoint.com/personal/dgutierrezv_sura_com/Documents/Documents/GitHub/macro/GDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{5C334686-4CE3-4EB5-8BDA-CC65A366C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34E7C006-51C5-4DBA-A963-9B6BEBEC4495}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5C334686-4CE3-4EB5-8BDA-CC65A366C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59542AC6-78DB-4419-9B24-EC11FDC084E7}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{38870D0C-4BAA-46FD-B714-AFC6A4ED00F5}"/>
   </bookViews>
@@ -57386,11 +57386,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CBE177-ED79-4759-AD45-50883F599728}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
add population growth prospect
</commit_message>
<xml_diff>
--- a/GDP/simple_golden_rule_pan.xlsx
+++ b/GDP/simple_golden_rule_pan.xlsx
@@ -57386,8 +57386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CBE177-ED79-4759-AD45-50883F599728}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
solow forecasted values for k and y
</commit_message>
<xml_diff>
--- a/GDP/simple_golden_rule_pan.xlsx
+++ b/GDP/simple_golden_rule_pan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana-my.sharepoint.com/personal/dgutierrezv_sura_com/Documents/Documents/GitHub/macro/GDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5C334686-4CE3-4EB5-8BDA-CC65A366C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59542AC6-78DB-4419-9B24-EC11FDC084E7}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{5C334686-4CE3-4EB5-8BDA-CC65A366C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98E7E400-7B1C-4171-B066-8BFA4C02AE72}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{38870D0C-4BAA-46FD-B714-AFC6A4ED00F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{38870D0C-4BAA-46FD-B714-AFC6A4ED00F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="615">
   <si>
     <t>Country Name</t>
   </si>
@@ -2010,6 +2010,12 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>y_growth</t>
+  </si>
+  <si>
+    <t>k_growth</t>
   </si>
 </sst>
 </file>
@@ -57384,18 +57390,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CBE177-ED79-4759-AD45-50883F599728}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>598</v>
       </c>
@@ -57427,10 +57433,16 @@
         <v>610</v>
       </c>
       <c r="K1" t="s">
+        <v>614</v>
+      </c>
+      <c r="L1" t="s">
+        <v>613</v>
+      </c>
+      <c r="M1" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -57462,7 +57474,7 @@
         <v>2083.3741121403095</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -57498,11 +57510,19 @@
         <v>0.10926594841623016</v>
       </c>
       <c r="K3" s="4">
+        <f>+G3/G2-1</f>
+        <v>0.23288829634901287</v>
+      </c>
+      <c r="L3" s="4">
+        <f>+H3/H2-1</f>
+        <v>7.6926309698267081E-2</v>
+      </c>
+      <c r="M3" s="4">
         <f>+D3/D2-1</f>
         <v>3.0029574379164314E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -57538,11 +57558,19 @@
         <v>8.2447368199746629E-2</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" ref="K4:K63" si="4">+D4/D3-1</f>
+        <f t="shared" ref="K4:K63" si="4">+G4/G3-1</f>
+        <v>9.320570938386985E-2</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4:L63" si="5">+H4/H3-1</f>
+        <v>5.0364538436822759E-2</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" ref="M4:M63" si="6">+D4/D3-1</f>
         <v>3.0544471551438912E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -57579,10 +57607,18 @@
       </c>
       <c r="K5" s="4">
         <f t="shared" si="4"/>
+        <v>9.0018244856195251E-2</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="5"/>
+        <v>5.2843861986439533E-2</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" si="6"/>
         <v>3.091059100267568E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -57619,10 +57655,18 @@
       </c>
       <c r="K6" s="4">
         <f t="shared" si="4"/>
+        <v>-0.1154671570310184</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="5"/>
+        <v>1.2950457174155439E-2</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="6"/>
         <v>3.0969773779724985E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -57659,10 +57703,18 @@
       </c>
       <c r="K7" s="4">
         <f t="shared" si="4"/>
+        <v>0.10095652962589963</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="5"/>
+        <v>5.9036995487315114E-2</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="6"/>
         <v>3.0748092155402418E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -57699,10 +57751,18 @@
       </c>
       <c r="K8" s="4">
         <f t="shared" si="4"/>
+        <v>0.29221270628795071</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="5"/>
+        <v>4.4023835739020356E-2</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="6"/>
         <v>3.0449671742375006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -57739,10 +57799,18 @@
       </c>
       <c r="K9" s="4">
         <f t="shared" si="4"/>
+        <v>2.4453144449914088E-2</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="5"/>
+        <v>5.3839115055445586E-2</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="6"/>
         <v>3.0071190451860241E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -57779,10 +57847,18 @@
       </c>
       <c r="K10" s="4">
         <f t="shared" si="4"/>
+        <v>9.9928503316114359E-2</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9013652929096976E-2</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="6"/>
         <v>2.9605225322628881E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -57819,10 +57895,18 @@
       </c>
       <c r="K11" s="4">
         <f t="shared" si="4"/>
+        <v>0.11245011765715973</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="5"/>
+        <v>5.3727339820975661E-2</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="6"/>
         <v>2.9121909157238113E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -57859,10 +57943,18 @@
       </c>
       <c r="K12" s="4">
         <f t="shared" si="4"/>
+        <v>0.1457673346209829</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9806117117286766E-2</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="6"/>
         <v>2.8645863368533142E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -57899,10 +57991,18 @@
       </c>
       <c r="K13" s="4">
         <f t="shared" si="4"/>
+        <v>0.19346854933391144</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="5"/>
+        <v>6.6010244573222243E-2</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="6"/>
         <v>2.828409141874233E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -57939,10 +58039,18 @@
       </c>
       <c r="K14" s="4">
         <f t="shared" si="4"/>
+        <v>0.11361652177208126</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="5"/>
+        <v>1.7393327398495639E-2</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="6"/>
         <v>2.7948677161798718E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -57979,10 +58087,18 @@
       </c>
       <c r="K15" s="4">
         <f t="shared" si="4"/>
+        <v>1.0359660495025791E-2</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="5"/>
+        <v>2.5529827353443668E-2</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="6"/>
         <v>2.7413415064836633E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -58019,10 +58135,18 @@
       </c>
       <c r="K16" s="4">
         <f t="shared" si="4"/>
+        <v>-7.5411992388646154E-2</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.2372469641461779E-3</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" si="6"/>
         <v>2.6780356860887311E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -58059,10 +58183,18 @@
       </c>
       <c r="K17" s="4">
         <f t="shared" si="4"/>
+        <v>-5.9892665872127937E-2</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="5"/>
+        <v>-8.511670486218037E-3</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="6"/>
         <v>2.6143388798326894E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -58099,10 +58231,18 @@
       </c>
       <c r="K18" s="4">
         <f t="shared" si="4"/>
+        <v>-3.4068777980666765E-2</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="5"/>
+        <v>-8.5915353872758615E-3</v>
+      </c>
+      <c r="M18" s="4">
+        <f t="shared" si="6"/>
         <v>2.545484518778296E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -58139,10 +58279,18 @@
       </c>
       <c r="K19" s="4">
         <f t="shared" si="4"/>
+        <v>-0.32152807159198737</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="5"/>
+        <v>-1.3518321964706703E-2</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="6"/>
         <v>2.4793750776403112E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -58179,10 +58327,18 @@
       </c>
       <c r="K20" s="4">
         <f t="shared" si="4"/>
+        <v>0.21940736140401884</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="5"/>
+        <v>7.1957511080514402E-2</v>
+      </c>
+      <c r="M20" s="4">
+        <f t="shared" si="6"/>
         <v>2.4225706553397286E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -58219,10 +58375,18 @@
       </c>
       <c r="K21" s="4">
         <f t="shared" si="4"/>
+        <v>5.298296905572375E-2</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="5"/>
+        <v>2.0819773174437506E-2</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="6"/>
         <v>2.3831569747546411E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -58259,10 +58423,18 @@
       </c>
       <c r="K22" s="4">
         <f t="shared" si="4"/>
+        <v>0.15171333289895994</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="5"/>
+        <v>0.10474160202566307</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="6"/>
         <v>2.3628344598376261E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -58299,10 +58471,18 @@
       </c>
       <c r="K23" s="4">
         <f t="shared" si="4"/>
+        <v>7.594436257686521E-2</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="5"/>
+        <v>6.6932055103472221E-2</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" si="6"/>
         <v>2.3559175405866162E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -58339,10 +58519,18 @@
       </c>
       <c r="K24" s="4">
         <f t="shared" si="4"/>
+        <v>-3.2430904446638653E-2</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="5"/>
+        <v>2.9254769323208141E-2</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" si="6"/>
         <v>2.3541105450972877E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -58379,10 +58567,18 @@
       </c>
       <c r="K25" s="4">
         <f t="shared" si="4"/>
+        <v>-0.3882281706476769</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="5"/>
+        <v>-6.6874495900032027E-2</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="6"/>
         <v>2.3534725328216544E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -58419,10 +58615,18 @@
       </c>
       <c r="K26" s="4">
         <f t="shared" si="4"/>
+        <v>-6.1427568157507939E-2</v>
+      </c>
+      <c r="L26" s="4">
+        <f t="shared" si="5"/>
+        <v>3.6228177303492259E-3</v>
+      </c>
+      <c r="M26" s="4">
+        <f t="shared" si="6"/>
         <v>2.3387192464709328E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -58459,10 +58663,18 @@
       </c>
       <c r="K27" s="4">
         <f t="shared" si="4"/>
+        <v>-6.2444810458616828E-2</v>
+      </c>
+      <c r="L27" s="4">
+        <f t="shared" si="5"/>
+        <v>2.5784523073615784E-2</v>
+      </c>
+      <c r="M27" s="4">
+        <f t="shared" si="6"/>
         <v>2.3043644069572267E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -58499,10 +58711,18 @@
       </c>
       <c r="K28" s="4">
         <f t="shared" si="4"/>
+        <v>0.25773069084321509</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="5"/>
+        <v>1.2680077275823098E-2</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="6"/>
         <v>2.2709842448903395E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -58539,10 +58759,18 @@
       </c>
       <c r="K29" s="4">
         <f t="shared" si="4"/>
+        <v>2.3743440176953179E-3</v>
+      </c>
+      <c r="L29" s="4">
+        <f t="shared" si="5"/>
+        <v>-3.9577975852124414E-2</v>
+      </c>
+      <c r="M29" s="4">
+        <f t="shared" si="6"/>
         <v>2.2372894933599063E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -58579,10 +58807,18 @@
       </c>
       <c r="K30" s="4">
         <f t="shared" si="4"/>
+        <v>-0.62595666624730484</v>
+      </c>
+      <c r="L30" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.1524630366313674</v>
+      </c>
+      <c r="M30" s="4">
+        <f t="shared" si="6"/>
         <v>2.2022164945536549E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -58619,10 +58855,18 @@
       </c>
       <c r="K31" s="4">
         <f t="shared" si="4"/>
+        <v>-0.28870132358031608</v>
+      </c>
+      <c r="L31" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.8515872118205525E-3</v>
+      </c>
+      <c r="M31" s="4">
+        <f t="shared" si="6"/>
         <v>2.1600454208391628E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -58659,10 +58903,18 @@
       </c>
       <c r="K32" s="4">
         <f t="shared" si="4"/>
+        <v>2.5260864027844154</v>
+      </c>
+      <c r="L32" s="4">
+        <f t="shared" si="5"/>
+        <v>5.8296345866571952E-2</v>
+      </c>
+      <c r="M32" s="4">
+        <f t="shared" si="6"/>
         <v>2.1443506140206514E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -58699,10 +58951,18 @@
       </c>
       <c r="K33" s="4">
         <f t="shared" si="4"/>
+        <v>8.2153270608700257E-2</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" si="5"/>
+        <v>7.141625894576098E-2</v>
+      </c>
+      <c r="M33" s="4">
+        <f t="shared" si="6"/>
         <v>2.1255787830698258E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -58739,10 +58999,18 @@
       </c>
       <c r="K34" s="4">
         <f t="shared" si="4"/>
+        <v>0.35794326572589408</v>
+      </c>
+      <c r="L34" s="4">
+        <f t="shared" si="5"/>
+        <v>5.9846824278881661E-2</v>
+      </c>
+      <c r="M34" s="4">
+        <f t="shared" si="6"/>
         <v>2.0918097363595622E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -58779,10 +59047,18 @@
       </c>
       <c r="K35" s="4">
         <f t="shared" si="4"/>
+        <v>0.11442725364178274</v>
+      </c>
+      <c r="L35" s="4">
+        <f t="shared" si="5"/>
+        <v>3.3075201113538677E-2</v>
+      </c>
+      <c r="M35" s="4">
+        <f t="shared" si="6"/>
         <v>2.0794462222173404E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -58819,10 +59095,18 @@
       </c>
       <c r="K36" s="4">
         <f t="shared" si="4"/>
+        <v>0.12003827334858519</v>
+      </c>
+      <c r="L36" s="4">
+        <f t="shared" si="5"/>
+        <v>7.6770364577856132E-3</v>
+      </c>
+      <c r="M36" s="4">
+        <f t="shared" si="6"/>
         <v>2.0665779737595313E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -58859,10 +59143,18 @@
       </c>
       <c r="K37" s="4">
         <f t="shared" si="4"/>
+        <v>8.566124182155388E-2</v>
+      </c>
+      <c r="L37" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.9686617855677611E-3</v>
+      </c>
+      <c r="M37" s="4">
+        <f t="shared" si="6"/>
         <v>2.054644480223633E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -58899,10 +59191,18 @@
       </c>
       <c r="K38" s="4">
         <f t="shared" si="4"/>
+        <v>5.3073089254206396E-2</v>
+      </c>
+      <c r="L38" s="4">
+        <f t="shared" si="5"/>
+        <v>1.9940955702326679E-2</v>
+      </c>
+      <c r="M38" s="4">
+        <f t="shared" si="6"/>
         <v>2.0448317364777813E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -58939,10 +59239,18 @@
       </c>
       <c r="K39" s="4">
         <f t="shared" si="4"/>
+        <v>2.1469189099374786E-2</v>
+      </c>
+      <c r="L39" s="4">
+        <f t="shared" si="5"/>
+        <v>4.3383149137363075E-2</v>
+      </c>
+      <c r="M39" s="4">
+        <f t="shared" si="6"/>
         <v>2.0344161471724354E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -58979,10 +59287,18 @@
       </c>
       <c r="K40" s="4">
         <f t="shared" si="4"/>
+        <v>8.7306707468487676E-2</v>
+      </c>
+      <c r="L40" s="4">
+        <f t="shared" si="5"/>
+        <v>5.2139626982177001E-2</v>
+      </c>
+      <c r="M40" s="4">
+        <f t="shared" si="6"/>
         <v>2.0221061445718336E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -59019,10 +59335,18 @@
       </c>
       <c r="K41" s="4">
         <f t="shared" si="4"/>
+        <v>1.5047741411986948E-2</v>
+      </c>
+      <c r="L41" s="4">
+        <f t="shared" si="5"/>
+        <v>1.8713251087444371E-2</v>
+      </c>
+      <c r="M41" s="4">
+        <f t="shared" si="6"/>
         <v>2.0082996641107353E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -59059,10 +59383,18 @@
       </c>
       <c r="K42" s="4">
         <f t="shared" si="4"/>
+        <v>-0.10986371140181495</v>
+      </c>
+      <c r="L42" s="4">
+        <f t="shared" si="5"/>
+        <v>7.0978111714805614E-3</v>
+      </c>
+      <c r="M42" s="4">
+        <f t="shared" si="6"/>
         <v>1.9914580445241858E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -59099,10 +59431,18 @@
       </c>
       <c r="K43" s="4">
         <f t="shared" si="4"/>
+        <v>-0.25649973553191596</v>
+      </c>
+      <c r="L43" s="4">
+        <f t="shared" si="5"/>
+        <v>-1.3738825837026458E-2</v>
+      </c>
+      <c r="M43" s="4">
+        <f t="shared" si="6"/>
         <v>1.9752935889325141E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -59139,10 +59479,18 @@
       </c>
       <c r="K44" s="4">
         <f t="shared" si="4"/>
+        <v>-7.2462876705618684E-2</v>
+      </c>
+      <c r="L44" s="4">
+        <f t="shared" si="5"/>
+        <v>2.6494152942262428E-3</v>
+      </c>
+      <c r="M44" s="4">
+        <f t="shared" si="6"/>
         <v>1.9590176359283618E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -59179,10 +59527,18 @@
       </c>
       <c r="K45" s="4">
         <f t="shared" si="4"/>
+        <v>0.16772235539925973</v>
+      </c>
+      <c r="L45" s="4">
+        <f t="shared" si="5"/>
+        <v>2.2201071875637801E-2</v>
+      </c>
+      <c r="M45" s="4">
+        <f t="shared" si="6"/>
         <v>1.9422683187065637E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -59219,10 +59575,18 @@
       </c>
       <c r="K46" s="4">
         <f t="shared" si="4"/>
+        <v>7.7757509983716444E-2</v>
+      </c>
+      <c r="L46" s="4">
+        <f t="shared" si="5"/>
+        <v>5.4765049716295255E-2</v>
+      </c>
+      <c r="M46" s="4">
+        <f t="shared" si="6"/>
         <v>1.9393652517846416E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -59259,10 +59623,18 @@
       </c>
       <c r="K47" s="4">
         <f t="shared" si="4"/>
+        <v>9.0018270766512032E-3</v>
+      </c>
+      <c r="L47" s="4">
+        <f t="shared" si="5"/>
+        <v>5.1628968820496279E-2</v>
+      </c>
+      <c r="M47" s="4">
+        <f t="shared" si="6"/>
         <v>1.9288005374754391E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -59299,10 +59671,18 @@
       </c>
       <c r="K48" s="4">
         <f t="shared" si="4"/>
+        <v>0.11425770532665225</v>
+      </c>
+      <c r="L48" s="4">
+        <f t="shared" si="5"/>
+        <v>6.6299317791459256E-2</v>
+      </c>
+      <c r="M48" s="4">
+        <f t="shared" si="6"/>
         <v>1.8967786977580392E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -59339,10 +59719,18 @@
       </c>
       <c r="K49" s="4">
         <f t="shared" si="4"/>
+        <v>0.36354499170653187</v>
+      </c>
+      <c r="L49" s="4">
+        <f t="shared" si="5"/>
+        <v>9.9267661319933032E-2</v>
+      </c>
+      <c r="M49" s="4">
+        <f t="shared" si="6"/>
         <v>1.8714452677736304E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -59379,10 +59767,18 @@
       </c>
       <c r="K50" s="4">
         <f t="shared" si="4"/>
+        <v>0.25862405165815772</v>
+      </c>
+      <c r="L50" s="4">
+        <f t="shared" si="5"/>
+        <v>7.854774034401224E-2</v>
+      </c>
+      <c r="M50" s="4">
+        <f t="shared" si="6"/>
         <v>1.8551620316271E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -59419,10 +59815,18 @@
       </c>
       <c r="K51" s="4">
         <f t="shared" si="4"/>
+        <v>-0.22814590421516523</v>
+      </c>
+      <c r="L51" s="4">
+        <f t="shared" si="5"/>
+        <v>-5.7934815035652898E-3</v>
+      </c>
+      <c r="M51" s="4">
+        <f t="shared" si="6"/>
         <v>1.8329596861592634E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -59459,10 +59863,18 @@
       </c>
       <c r="K52" s="4">
         <f t="shared" si="4"/>
+        <v>0.30497854715285566</v>
+      </c>
+      <c r="L52" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9508667301018097E-2</v>
+      </c>
+      <c r="M52" s="4">
+        <f t="shared" si="6"/>
         <v>1.8057826964133605E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -59499,10 +59911,18 @@
       </c>
       <c r="K53" s="4">
         <f t="shared" si="4"/>
+        <v>0.11776292170085179</v>
+      </c>
+      <c r="L53" s="4">
+        <f t="shared" si="5"/>
+        <v>9.3503918150657617E-2</v>
+      </c>
+      <c r="M53" s="4">
+        <f t="shared" si="6"/>
         <v>1.7953608231775053E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -59539,10 +59959,18 @@
       </c>
       <c r="K54" s="4">
         <f t="shared" si="4"/>
+        <v>0.23149073436423406</v>
+      </c>
+      <c r="L54" s="4">
+        <f t="shared" si="5"/>
+        <v>7.8433940010694814E-2</v>
+      </c>
+      <c r="M54" s="4">
+        <f t="shared" si="6"/>
         <v>1.794357538779523E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -59579,10 +60007,18 @@
       </c>
       <c r="K55" s="4">
         <f t="shared" si="4"/>
+        <v>8.5798194128019922E-2</v>
+      </c>
+      <c r="L55" s="4">
+        <f t="shared" si="5"/>
+        <v>5.0382546241173332E-2</v>
+      </c>
+      <c r="M55" s="4">
+        <f t="shared" si="6"/>
         <v>1.7762037592859548E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -59619,10 +60055,18 @@
       </c>
       <c r="K56" s="4">
         <f t="shared" si="4"/>
+        <v>4.3092100263840916E-2</v>
+      </c>
+      <c r="L56" s="4">
+        <f t="shared" si="5"/>
+        <v>3.2498301523364859E-2</v>
+      </c>
+      <c r="M56" s="4">
+        <f t="shared" si="6"/>
         <v>1.7594142281311509E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -59659,10 +60103,18 @@
       </c>
       <c r="K57" s="4">
         <f t="shared" si="4"/>
+        <v>4.6050696581585004E-2</v>
+      </c>
+      <c r="L57" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9079288678276036E-2</v>
+      </c>
+      <c r="M57" s="4">
+        <f t="shared" si="6"/>
         <v>1.7564833098598909E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -59699,10 +60151,18 @@
       </c>
       <c r="K58" s="4">
         <f t="shared" si="4"/>
+        <v>-2.1786896937026734E-2</v>
+      </c>
+      <c r="L58" s="4">
+        <f t="shared" si="5"/>
+        <v>3.1484327110090193E-2</v>
+      </c>
+      <c r="M58" s="4">
+        <f t="shared" si="6"/>
         <v>1.7496908720251891E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -59739,10 +60199,18 @@
       </c>
       <c r="K59" s="4">
         <f t="shared" si="4"/>
+        <v>6.3812440847049734E-2</v>
+      </c>
+      <c r="L59" s="4">
+        <f t="shared" si="5"/>
+        <v>3.793677977836607E-2</v>
+      </c>
+      <c r="M59" s="4">
+        <f t="shared" si="6"/>
         <v>1.7317730065250281E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -59779,10 +60247,18 @@
       </c>
       <c r="K60" s="4">
         <f t="shared" si="4"/>
+        <v>3.8560585127087599E-3</v>
+      </c>
+      <c r="L60" s="4">
+        <f t="shared" si="5"/>
+        <v>1.9630378470624432E-2</v>
+      </c>
+      <c r="M60" s="4">
+        <f t="shared" si="6"/>
         <v>1.6892318306627629E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -59819,10 +60295,18 @@
       </c>
       <c r="K61" s="4">
         <f t="shared" si="4"/>
+        <v>-6.0277032477103032E-2</v>
+      </c>
+      <c r="L61" s="4">
+        <f t="shared" si="5"/>
+        <v>1.3428865340273211E-2</v>
+      </c>
+      <c r="M61" s="4">
+        <f t="shared" si="6"/>
         <v>1.6151952281432846E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -59859,10 +60343,18 @@
       </c>
       <c r="K62" s="4">
         <f t="shared" si="4"/>
+        <v>-0.50845742838271601</v>
+      </c>
+      <c r="L62" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.1912695903846614</v>
+      </c>
+      <c r="M62" s="4">
+        <f t="shared" si="6"/>
         <v>1.4616310047980807E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -59899,6 +60391,14 @@
       </c>
       <c r="K63" s="4">
         <f t="shared" si="4"/>
+        <v>0.28917893983492204</v>
+      </c>
+      <c r="L63" s="4">
+        <f t="shared" si="5"/>
+        <v>0.13828435638977443</v>
+      </c>
+      <c r="M63" s="4">
+        <f t="shared" si="6"/>
         <v>1.3243073065455579E-2</v>
       </c>
     </row>

</xml_diff>